<commit_message>
Mark That Pawn 업데이트
#241
</commit_message>
<xml_diff>
--- a/Data/Mlie/Mark That Pawn - 3056996662/3056996662.xlsx
+++ b/Data/Mlie/Mark That Pawn - 3056996662/3056996662.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\Mark That Pawn - 3056996662\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\Mark.That.Pawn.-.3056996662\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B955BB0-39F0-4E99-9568-7D598BA633DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E164A0-32D1-4EA6-97BE-A0663AEEB8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Update" sheetId="2" r:id="rId2"/>
+    <sheet name="Update_231204" sheetId="3" r:id="rId2"/>
+    <sheet name="Update" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="517">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1440,8 +1441,155 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Update [Not chosen]</t>
+    <t>Keyed+MTP.DuplicateRule</t>
+  </si>
+  <si>
+    <t>규칙 복사</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.Male</t>
+  </si>
+  <si>
+    <t>남성</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.Female</t>
+  </si>
+  <si>
+    <t>여성</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.Animal</t>
+  </si>
+  <si>
+    <t>동물</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.OnlyAnimal</t>
+  </si>
+  <si>
+    <t>동물임</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.NotAnimal</t>
+  </si>
+  <si>
+    <t>동물 아님</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.LowAgeLimit</t>
+  </si>
+  <si>
+    <t>최소 나이 제한: {0}</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.HighAgeLimit</t>
+  </si>
+  <si>
+    <t>최대 나이 제한: {0}</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.Unlimited</t>
+  </si>
+  <si>
+    <t>최대 나이 제한: 제한 없음</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.AutomaticType.Animal</t>
+  </si>
+  <si>
+    <t>특정 동물인 폰</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.AutomaticType.Gender</t>
+  </si>
+  <si>
+    <t>특정 성별인 폰</t>
+  </si>
+  <si>
+    <t>Keyed+MTP.AutomaticType.Age</t>
+  </si>
+  <si>
+    <t>특정 나이대의 폰</t>
+  </si>
+  <si>
+    <t>직업 지정을 나타내는 마커, 제작자: [✚] Survivalmaster</t>
+  </si>
+  <si>
+    <t>Update_231204 [Not chosen]</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTP.DuplicateRule</t>
+  </si>
+  <si>
+    <t>MTP.Male</t>
+  </si>
+  <si>
+    <t>MTP.Female</t>
+  </si>
+  <si>
+    <t>MTP.Animal</t>
+  </si>
+  <si>
+    <t>MTP.OnlyAnimal</t>
+  </si>
+  <si>
+    <t>MTP.NotAnimal</t>
+  </si>
+  <si>
+    <t>MTP.LowAgeLimit</t>
+  </si>
+  <si>
+    <t>MTP.HighAgeLimit</t>
+  </si>
+  <si>
+    <t>MTP.Unlimited</t>
+  </si>
+  <si>
+    <t>MTP.AutomaticType.Animal</t>
+  </si>
+  <si>
+    <t>MTP.AutomaticType.Gender</t>
+  </si>
+  <si>
+    <t>MTP.AutomaticType.Age</t>
+  </si>
+  <si>
+    <t>Duplicate rule</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Animals</t>
+  </si>
+  <si>
+    <t>Only animals</t>
+  </si>
+  <si>
+    <t>Not animals</t>
+  </si>
+  <si>
+    <t>Low age-limit: {0}</t>
+  </si>
+  <si>
+    <t>High age-limit: {0}</t>
+  </si>
+  <si>
+    <t>High age-limit: No limit</t>
+  </si>
+  <si>
+    <t>Pawn is a specific animal</t>
+  </si>
+  <si>
+    <t>Pawn is of specified gender</t>
+  </si>
+  <si>
+    <t>Pawn is in specified age-range</t>
   </si>
 </sst>
 </file>
@@ -1866,10 +2014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1880,7 +2028,7 @@
     <col min="4" max="4" width="32.75" customWidth="1"/>
     <col min="5" max="5" width="40.25" customWidth="1"/>
     <col min="6" max="6" width="28.08203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.4140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -1903,7 +2051,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>467</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1926,7 +2074,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="str">
-        <f>IFERROR(VLOOKUP(A2,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A2,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>WOW 스타일</v>
       </c>
     </row>
@@ -1950,7 +2098,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="str">
-        <f>IFERROR(VLOOKUP(A3,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A3,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>월드 오브 워크래프트의 공격대 마커에서 영감을 얻은 마커</v>
       </c>
     </row>
@@ -1974,7 +2122,7 @@
         <v>18</v>
       </c>
       <c r="G4" t="str">
-        <f>IFERROR(VLOOKUP(A4,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A4,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>숫자</v>
       </c>
     </row>
@@ -1998,7 +2146,7 @@
         <v>22</v>
       </c>
       <c r="G5" t="str">
-        <f>IFERROR(VLOOKUP(A5,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A5,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>간단하게 번호를 매길 수 있는 마커</v>
       </c>
     </row>
@@ -2019,7 +2167,7 @@
         <v>446</v>
       </c>
       <c r="G6" t="str">
-        <f>IFERROR(VLOOKUP(A6,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A6,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>기술</v>
       </c>
     </row>
@@ -2040,7 +2188,7 @@
         <v>447</v>
       </c>
       <c r="G7" t="str">
-        <f>IFERROR(VLOOKUP(A7,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A7,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>업무 기술을 나타내는 마커</v>
       </c>
     </row>
@@ -2061,7 +2209,7 @@
         <v>448</v>
       </c>
       <c r="G8" t="str">
-        <f>IFERROR(VLOOKUP(A8,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A8,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>직업</v>
       </c>
     </row>
@@ -2082,8 +2230,8 @@
         <v>449</v>
       </c>
       <c r="G9" t="str">
-        <f>IFERROR(VLOOKUP(A9,Update!$C$2:$D$115,2,FALSE),"")</f>
-        <v>직업 지정을 나타내는 마커, 제작자: [?] Survivalmaster</v>
+        <f>IFERROR(VLOOKUP(A9,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>직업 지정을 나타내는 마커, 제작자: [✚] Survivalmaster</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -2103,7 +2251,7 @@
         <v>450</v>
       </c>
       <c r="G10" t="str">
-        <f>IFERROR(VLOOKUP(A10,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A10,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>군대</v>
       </c>
     </row>
@@ -2124,7 +2272,7 @@
         <v>451</v>
       </c>
       <c r="G11" t="str">
-        <f>IFERROR(VLOOKUP(A11,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A11,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>미군을 기반으로 한 마커</v>
       </c>
     </row>
@@ -2145,7 +2293,7 @@
         <v>43</v>
       </c>
       <c r="G12" t="str">
-        <f>IFERROR(VLOOKUP(A12,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A12,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>GDI</v>
       </c>
     </row>
@@ -2166,7 +2314,7 @@
         <v>452</v>
       </c>
       <c r="G13" t="str">
-        <f>IFERROR(VLOOKUP(A13,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A13,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>게임 커맨드 앤 컨커의 GDI 진영을 기반으로 한 마커입니다.</v>
       </c>
     </row>
@@ -2187,7 +2335,7 @@
         <v>49</v>
       </c>
       <c r="G14" t="str">
-        <f>IFERROR(VLOOKUP(A14,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A14,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>Nod</v>
       </c>
     </row>
@@ -2208,7 +2356,7 @@
         <v>453</v>
       </c>
       <c r="G15" t="str">
-        <f>IFERROR(VLOOKUP(A15,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A15,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>게임 커맨드 앤 컨커의 Nod 진영을 기반으로 한 마커입니다.</v>
       </c>
     </row>
@@ -2229,7 +2377,7 @@
         <v>55</v>
       </c>
       <c r="G16" t="str">
-        <f>IFERROR(VLOOKUP(A16,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A16,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>XCOM</v>
       </c>
     </row>
@@ -2250,7 +2398,7 @@
         <v>454</v>
       </c>
       <c r="G17" t="str">
-        <f>IFERROR(VLOOKUP(A17,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A17,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>게임 XCOM을 기반으로 한 마커, 제작자: Botaxalim</v>
       </c>
     </row>
@@ -2271,7 +2419,7 @@
         <v>61</v>
       </c>
       <c r="G18" t="str">
-        <f>IFERROR(VLOOKUP(A18,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A18,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>XCOM 2</v>
       </c>
     </row>
@@ -2292,7 +2440,7 @@
         <v>461</v>
       </c>
       <c r="G19" t="str">
-        <f>IFERROR(VLOOKUP(A19,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A19,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>레코다의 게임 XCOM 2를 기반으로 한 귀여운 마커</v>
       </c>
     </row>
@@ -2313,7 +2461,7 @@
         <v>455</v>
       </c>
       <c r="G20" t="str">
-        <f>IFERROR(VLOOKUP(A20,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A20,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>무기</v>
       </c>
     </row>
@@ -2334,7 +2482,7 @@
         <v>456</v>
       </c>
       <c r="G21" t="str">
-        <f>IFERROR(VLOOKUP(A21,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A21,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>일반 무기 유형, 제작자: flaticon.com의 max.icons</v>
       </c>
     </row>
@@ -2355,7 +2503,7 @@
         <v>457</v>
       </c>
       <c r="G22" t="str">
-        <f>IFERROR(VLOOKUP(A22,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A22,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>XCOM 중세</v>
       </c>
     </row>
@@ -2376,7 +2524,7 @@
         <v>458</v>
       </c>
       <c r="G23" t="str">
-        <f>IFERROR(VLOOKUP(A23,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A23,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>XCOM 게임을 기반으로 한 중세 스타일의 마커, 제작자: Botaxalim</v>
       </c>
     </row>
@@ -2397,7 +2545,7 @@
         <v>462</v>
       </c>
       <c r="G24" t="str">
-        <f>IFERROR(VLOOKUP(A24,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A24,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>심볼</v>
       </c>
     </row>
@@ -2418,7 +2566,7 @@
         <v>463</v>
       </c>
       <c r="G25" t="str">
-        <f>IFERROR(VLOOKUP(A25,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A25,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>일반적인 기호를 사용한 마커</v>
       </c>
     </row>
@@ -2439,7 +2587,7 @@
         <v>459</v>
       </c>
       <c r="G26" t="str">
-        <f>IFERROR(VLOOKUP(A26,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A26,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>이데올로기</v>
       </c>
     </row>
@@ -2460,7 +2608,7 @@
         <v>460</v>
       </c>
       <c r="G27" t="str">
-        <f>IFERROR(VLOOKUP(A27,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A27,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>이데올로기의 마커, 제작자: Yoann</v>
       </c>
     </row>
@@ -2481,7 +2629,7 @@
         <v>354</v>
       </c>
       <c r="G28" t="str">
-        <f>IFERROR(VLOOKUP(A28,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A28,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>설치된 모드 버전: {0}</v>
       </c>
     </row>
@@ -2502,7 +2650,7 @@
         <v>355</v>
       </c>
       <c r="G29" t="str">
-        <f>IFERROR(VLOOKUP(A29,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A29,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>기본 마커 세트: {0}</v>
       </c>
     </row>
@@ -2523,7 +2671,7 @@
         <v>356</v>
       </c>
       <c r="G30" t="str">
-        <f>IFERROR(VLOOKUP(A30,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A30,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>정착민 마커 세트: {0}</v>
       </c>
     </row>
@@ -2544,7 +2692,7 @@
         <v>357</v>
       </c>
       <c r="G31" t="str">
-        <f>IFERROR(VLOOKUP(A31,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A31,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v xml:space="preserve">    정착민을 위한 다른 세트</v>
       </c>
     </row>
@@ -2565,7 +2713,7 @@
         <v>358</v>
       </c>
       <c r="G32" t="str">
-        <f>IFERROR(VLOOKUP(A32,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A32,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>정착민 설정 표시</v>
       </c>
     </row>
@@ -2586,7 +2734,7 @@
         <v>359</v>
       </c>
       <c r="G33" t="str">
-        <f>IFERROR(VLOOKUP(A33,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A33,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>포로 마커 세트: {0}</v>
       </c>
     </row>
@@ -2607,7 +2755,7 @@
         <v>360</v>
       </c>
       <c r="G34" t="str">
-        <f>IFERROR(VLOOKUP(A34,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A34,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v xml:space="preserve">    죄수를 위한 다른 세트</v>
       </c>
     </row>
@@ -2628,7 +2776,7 @@
         <v>361</v>
       </c>
       <c r="G35" t="str">
-        <f>IFERROR(VLOOKUP(A35,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A35,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>포로 설정 표시</v>
       </c>
     </row>
@@ -2649,7 +2797,7 @@
         <v>362</v>
       </c>
       <c r="G36" t="str">
-        <f>IFERROR(VLOOKUP(A36,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A36,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>노예 마커 세트: {0}</v>
       </c>
     </row>
@@ -2670,7 +2818,7 @@
         <v>363</v>
       </c>
       <c r="G37" t="str">
-        <f>IFERROR(VLOOKUP(A37,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A37,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v xml:space="preserve">    노예를 위한 다른 세트</v>
       </c>
     </row>
@@ -2691,7 +2839,7 @@
         <v>364</v>
       </c>
       <c r="G38" t="str">
-        <f>IFERROR(VLOOKUP(A38,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A38,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>노예 설정 표시</v>
       </c>
     </row>
@@ -2712,7 +2860,7 @@
         <v>365</v>
       </c>
       <c r="G39" t="str">
-        <f>IFERROR(VLOOKUP(A39,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A39,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>적 마커 세트: {0}</v>
       </c>
     </row>
@@ -2733,7 +2881,7 @@
         <v>366</v>
       </c>
       <c r="G40" t="str">
-        <f>IFERROR(VLOOKUP(A40,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A40,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v xml:space="preserve">    적을 위한 다른 세트</v>
       </c>
     </row>
@@ -2754,7 +2902,7 @@
         <v>367</v>
       </c>
       <c r="G41" t="str">
-        <f>IFERROR(VLOOKUP(A41,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A41,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>적 설정 표시</v>
       </c>
     </row>
@@ -2775,7 +2923,7 @@
         <v>368</v>
       </c>
       <c r="G42" t="str">
-        <f>IFERROR(VLOOKUP(A42,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A42,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>중립 마커 세트: {0}</v>
       </c>
     </row>
@@ -2796,7 +2944,7 @@
         <v>369</v>
       </c>
       <c r="G43" t="str">
-        <f>IFERROR(VLOOKUP(A43,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A43,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v xml:space="preserve">    중립을 위한 다른 세트</v>
       </c>
     </row>
@@ -2817,7 +2965,7 @@
         <v>370</v>
       </c>
       <c r="G44" t="str">
-        <f>IFERROR(VLOOKUP(A44,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A44,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>중립 설정 표시</v>
       </c>
     </row>
@@ -2838,7 +2986,7 @@
         <v>371</v>
       </c>
       <c r="G45" t="str">
-        <f>IFERROR(VLOOKUP(A45,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A45,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>차량 마커 세트: {0}</v>
       </c>
     </row>
@@ -2859,7 +3007,7 @@
         <v>372</v>
       </c>
       <c r="G46" t="str">
-        <f>IFERROR(VLOOKUP(A46,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A46,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v xml:space="preserve">    차량을 위한 다른 세트</v>
       </c>
     </row>
@@ -2880,7 +3028,7 @@
         <v>373</v>
       </c>
       <c r="G47" t="str">
-        <f>IFERROR(VLOOKUP(A47,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A47,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>차량 설정 표시</v>
       </c>
     </row>
@@ -2901,7 +3049,7 @@
         <v>374</v>
       </c>
       <c r="G48" t="str">
-        <f>IFERROR(VLOOKUP(A48,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A48,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>마커 선택</v>
       </c>
     </row>
@@ -2922,7 +3070,7 @@
         <v>375</v>
       </c>
       <c r="G49" t="str">
-        <f>IFERROR(VLOOKUP(A49,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A49,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>이 폰에 마커 추가</v>
       </c>
     </row>
@@ -2943,7 +3091,7 @@
         <v>376</v>
       </c>
       <c r="G50" t="str">
-        <f>IFERROR(VLOOKUP(A50,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A50,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>축소 시 아이콘 크기 확대</v>
       </c>
     </row>
@@ -2964,7 +3112,7 @@
         <v>377</v>
       </c>
       <c r="G51" t="str">
-        <f>IFERROR(VLOOKUP(A51,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A51,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>축소할 때 아이콘 크기를 늘려 더 잘 보이도록 합니다.</v>
       </c>
     </row>
@@ -2985,7 +3133,7 @@
         <v>378</v>
       </c>
       <c r="G52" t="str">
-        <f>IFERROR(VLOOKUP(A52,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A52,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>폰 크기에 따른 상대적 아이콘 크기</v>
       </c>
     </row>
@@ -3006,7 +3154,7 @@
         <v>379</v>
       </c>
       <c r="G53" t="str">
-        <f>IFERROR(VLOOKUP(A53,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A53,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>폰 크기에 따라 아이콘의 상대적 크기를 변경합니다.</v>
       </c>
     </row>
@@ -3027,7 +3175,7 @@
         <v>380</v>
       </c>
       <c r="G54" t="str">
-        <f>IFERROR(VLOOKUP(A54,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A54,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>저장되지 않은 규칙이 있습니다. 닫기 전에 변경 사항을 저장하시겠습니까?</v>
       </c>
     </row>
@@ -3048,7 +3196,7 @@
         <v>381</v>
       </c>
       <c r="G55" t="str">
-        <f>IFERROR(VLOOKUP(A55,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A55,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>규칙 초기화</v>
       </c>
     </row>
@@ -3069,7 +3217,7 @@
         <v>382</v>
       </c>
       <c r="G56" t="str">
-        <f>IFERROR(VLOOKUP(A56,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A56,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>정의된 모든 규칙을 정말 제거할까요?</v>
       </c>
     </row>
@@ -3090,7 +3238,7 @@
         <v>383</v>
       </c>
       <c r="G57" t="str">
-        <f>IFERROR(VLOOKUP(A57,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A57,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>선택되지 않음</v>
       </c>
     </row>
@@ -3111,7 +3259,7 @@
         <v>384</v>
       </c>
       <c r="G58" t="str">
-        <f>IFERROR(VLOOKUP(A58,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A58,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>{0} 선택됨</v>
       </c>
     </row>
@@ -3132,7 +3280,7 @@
         <v>385</v>
       </c>
       <c r="G59" t="str">
-        <f>IFERROR(VLOOKUP(A59,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A59,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>특성 변경</v>
       </c>
     </row>
@@ -3153,7 +3301,7 @@
         <v>386</v>
       </c>
       <c r="G60" t="str">
-        <f>IFERROR(VLOOKUP(A60,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A60,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>기술 변경</v>
       </c>
     </row>
@@ -3174,7 +3322,7 @@
         <v>387</v>
       </c>
       <c r="G61" t="str">
-        <f>IFERROR(VLOOKUP(A61,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A61,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>사용자 지정 아이콘</v>
       </c>
     </row>
@@ -3195,7 +3343,7 @@
         <v>388</v>
       </c>
       <c r="G62" t="str">
-        <f>IFERROR(VLOOKUP(A62,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A62,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>활성화</v>
       </c>
     </row>
@@ -3216,7 +3364,7 @@
         <v>389</v>
       </c>
       <c r="G63" t="str">
-        <f>IFERROR(VLOOKUP(A63,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A63,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>규칙 활성화, 비활성화하려면 클릭</v>
       </c>
     </row>
@@ -3237,7 +3385,7 @@
         <v>390</v>
       </c>
       <c r="G64" t="str">
-        <f>IFERROR(VLOOKUP(A64,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A64,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>비활성화</v>
       </c>
     </row>
@@ -3258,7 +3406,7 @@
         <v>391</v>
       </c>
       <c r="G65" t="str">
-        <f>IFERROR(VLOOKUP(A65,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A65,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>설정이 누락되어 규칙을 활성화할 수 없습니다.</v>
       </c>
     </row>
@@ -3279,7 +3427,7 @@
         <v>392</v>
       </c>
       <c r="G66" t="str">
-        <f>IFERROR(VLOOKUP(A66,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A66,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>규칙 비활성화, 활성화하려면 클릭</v>
       </c>
     </row>
@@ -3300,7 +3448,7 @@
         <v>393</v>
       </c>
       <c r="G67" t="str">
-        <f>IFERROR(VLOOKUP(A67,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A67,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>우선 순위 높이기</v>
       </c>
     </row>
@@ -3321,7 +3469,7 @@
         <v>394</v>
       </c>
       <c r="G68" t="str">
-        <f>IFERROR(VLOOKUP(A68,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A68,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>우선순위 낮추기</v>
       </c>
     </row>
@@ -3342,7 +3490,7 @@
         <v>395</v>
       </c>
       <c r="G69" t="str">
-        <f>IFERROR(VLOOKUP(A69,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A69,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>저장</v>
       </c>
     </row>
@@ -3363,7 +3511,7 @@
         <v>396</v>
       </c>
       <c r="G70" t="str">
-        <f>IFERROR(VLOOKUP(A70,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A70,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>취소</v>
       </c>
     </row>
@@ -3384,7 +3532,7 @@
         <v>397</v>
       </c>
       <c r="G71" t="str">
-        <f>IFERROR(VLOOKUP(A71,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A71,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>편집</v>
       </c>
     </row>
@@ -3405,7 +3553,7 @@
         <v>398</v>
       </c>
       <c r="G72" t="str">
-        <f>IFERROR(VLOOKUP(A72,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A72,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>삭제</v>
       </c>
     </row>
@@ -3426,7 +3574,7 @@
         <v>399</v>
       </c>
       <c r="G73" t="str">
-        <f>IFERROR(VLOOKUP(A73,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A73,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>정말 규칙을 삭제할까요?</v>
       </c>
     </row>
@@ -3447,7 +3595,7 @@
         <v>400</v>
       </c>
       <c r="G74" t="str">
-        <f>IFERROR(VLOOKUP(A74,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A74,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>자동 마킹 규칙</v>
       </c>
     </row>
@@ -3468,7 +3616,7 @@
         <v>401</v>
       </c>
       <c r="G75" t="str">
-        <f>IFERROR(VLOOKUP(A75,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A75,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>새 규칙</v>
       </c>
     </row>
@@ -3489,7 +3637,7 @@
         <v>402</v>
       </c>
       <c r="G76" t="str">
-        <f>IFERROR(VLOOKUP(A76,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A76,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>자동 규칙({0} 활성화됨)</v>
       </c>
     </row>
@@ -3510,7 +3658,7 @@
         <v>403</v>
       </c>
       <c r="G77" t="str">
-        <f>IFERROR(VLOOKUP(A77,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A77,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>규칙 편집</v>
       </c>
     </row>
@@ -3531,7 +3679,7 @@
         <v>404</v>
       </c>
       <c r="G78" t="str">
-        <f>IFERROR(VLOOKUP(A78,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A78,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>자동 아이콘</v>
       </c>
     </row>
@@ -3552,7 +3700,7 @@
         <v>430</v>
       </c>
       <c r="G79" t="str">
-        <f>IFERROR(VLOOKUP(A79,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A79,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>자동 아이콘 초기화</v>
       </c>
     </row>
@@ -3573,7 +3721,7 @@
         <v>405</v>
       </c>
       <c r="G80" t="str">
-        <f>IFERROR(VLOOKUP(A80,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A80,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>마커 없음</v>
       </c>
     </row>
@@ -3594,7 +3742,7 @@
         <v>406</v>
       </c>
       <c r="G81" t="str">
-        <f>IFERROR(VLOOKUP(A81,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A81,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>모든 값 초기화</v>
       </c>
     </row>
@@ -3615,7 +3763,7 @@
         <v>407</v>
       </c>
       <c r="G82" t="str">
-        <f>IFERROR(VLOOKUP(A82,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A82,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>수직 오프셋: {0}</v>
       </c>
     </row>
@@ -3636,7 +3784,7 @@
         <v>408</v>
       </c>
       <c r="G83" t="str">
-        <f>IFERROR(VLOOKUP(A83,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A83,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>수평 오프셋: {0}</v>
       </c>
     </row>
@@ -3657,7 +3805,7 @@
         <v>409</v>
       </c>
       <c r="G84" t="str">
-        <f>IFERROR(VLOOKUP(A84,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A84,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>마커 {0}</v>
       </c>
     </row>
@@ -3678,7 +3826,7 @@
         <v>410</v>
       </c>
       <c r="G85" t="str">
-        <f>IFERROR(VLOOKUP(A85,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A85,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>아이콘 크기: {0}</v>
       </c>
     </row>
@@ -3699,7 +3847,7 @@
         <v>411</v>
       </c>
       <c r="G86" t="str">
-        <f>IFERROR(VLOOKUP(A86,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A86,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v xml:space="preserve">    아이콘 확대/축소 배율: {0}</v>
       </c>
     </row>
@@ -3720,7 +3868,7 @@
         <v>412</v>
       </c>
       <c r="G87" t="str">
-        <f>IFERROR(VLOOKUP(A87,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A87,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>진동 아이콘 사용</v>
       </c>
     </row>
@@ -3741,7 +3889,7 @@
         <v>413</v>
       </c>
       <c r="G88" t="str">
-        <f>IFERROR(VLOOKUP(A88,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A88,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>아이콘은 상인 질문 마크와 같은 방식으로 진동합니다.</v>
       </c>
     </row>
@@ -3762,7 +3910,7 @@
         <v>414</v>
       </c>
       <c r="G89" t="str">
-        <f>IFERROR(VLOOKUP(A89,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A89,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>근접 무기</v>
       </c>
     </row>
@@ -3783,7 +3931,7 @@
         <v>415</v>
       </c>
       <c r="G90" t="str">
-        <f>IFERROR(VLOOKUP(A90,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A90,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>원거리 투사체 무기</v>
       </c>
     </row>
@@ -3804,7 +3952,7 @@
         <v>416</v>
       </c>
       <c r="G91" t="str">
-        <f>IFERROR(VLOOKUP(A91,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A91,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>원거리 폭발 무기</v>
       </c>
     </row>
@@ -3825,7 +3973,7 @@
         <v>417</v>
       </c>
       <c r="G92" t="str">
-        <f>IFERROR(VLOOKUP(A92,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A92,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>투척</v>
       </c>
     </row>
@@ -3846,7 +3994,7 @@
         <v>418</v>
       </c>
       <c r="G93" t="str">
-        <f>IFERROR(VLOOKUP(A93,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A93,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>정착민</v>
       </c>
     </row>
@@ -3867,7 +4015,7 @@
         <v>419</v>
       </c>
       <c r="G94" t="str">
-        <f>IFERROR(VLOOKUP(A94,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A94,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>노예</v>
       </c>
     </row>
@@ -3888,7 +4036,7 @@
         <v>420</v>
       </c>
       <c r="G95" t="str">
-        <f>IFERROR(VLOOKUP(A95,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A95,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>포로</v>
       </c>
     </row>
@@ -3909,7 +4057,7 @@
         <v>421</v>
       </c>
       <c r="G96" t="str">
-        <f>IFERROR(VLOOKUP(A96,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A96,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>차량</v>
       </c>
     </row>
@@ -3930,7 +4078,7 @@
         <v>422</v>
       </c>
       <c r="G97" t="str">
-        <f>IFERROR(VLOOKUP(A97,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A97,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>적</v>
       </c>
     </row>
@@ -3951,7 +4099,7 @@
         <v>423</v>
       </c>
       <c r="G98" t="str">
-        <f>IFERROR(VLOOKUP(A98,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A98,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>중립</v>
       </c>
     </row>
@@ -3972,7 +4120,7 @@
         <v>431</v>
       </c>
       <c r="G99" t="str">
-        <f>IFERROR(VLOOKUP(A99,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A99,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>모두</v>
       </c>
     </row>
@@ -3993,7 +4141,7 @@
         <v>424</v>
       </c>
       <c r="G100" t="str">
-        <f>IFERROR(VLOOKUP(A100,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A100,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>장착한 무기</v>
       </c>
     </row>
@@ -4014,7 +4162,7 @@
         <v>425</v>
       </c>
       <c r="G101" t="str">
-        <f>IFERROR(VLOOKUP(A101,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A101,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>장착 무기 유형</v>
       </c>
     </row>
@@ -4035,7 +4183,7 @@
         <v>426</v>
       </c>
       <c r="G102" t="str">
-        <f>IFERROR(VLOOKUP(A102,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A102,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>특성 보유</v>
       </c>
     </row>
@@ -4056,7 +4204,7 @@
         <v>427</v>
       </c>
       <c r="G103" t="str">
-        <f>IFERROR(VLOOKUP(A103,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A103,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>최소 기술</v>
       </c>
     </row>
@@ -4077,7 +4225,7 @@
         <v>428</v>
       </c>
       <c r="G104" t="str">
-        <f>IFERROR(VLOOKUP(A104,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A104,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>정착민과 관계 있음</v>
       </c>
     </row>
@@ -4098,7 +4246,7 @@
         <v>429</v>
       </c>
       <c r="G105" t="str">
-        <f>IFERROR(VLOOKUP(A105,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A105,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>폰의 유형</v>
       </c>
     </row>
@@ -4119,7 +4267,7 @@
         <v>432</v>
       </c>
       <c r="G106" t="str">
-        <f>IFERROR(VLOOKUP(A106,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A106,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>소집된 폰</v>
       </c>
     </row>
@@ -4140,7 +4288,7 @@
         <v>433</v>
       </c>
       <c r="G107" t="str">
-        <f>IFERROR(VLOOKUP(A107,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A107,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>폰의 정신 상태</v>
       </c>
     </row>
@@ -4161,7 +4309,7 @@
         <v>434</v>
       </c>
       <c r="G108" t="str">
-        <f>IFERROR(VLOOKUP(A108,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A108,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>일시적인 헤디프를 가진 폰</v>
       </c>
     </row>
@@ -4182,7 +4330,7 @@
         <v>435</v>
       </c>
       <c r="G109" t="str">
-        <f>IFERROR(VLOOKUP(A109,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A109,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>영구적인 헤디프를 가진 폰</v>
       </c>
     </row>
@@ -4203,113 +4351,365 @@
         <v>436</v>
       </c>
       <c r="G110" t="str">
-        <f>IFERROR(VLOOKUP(A110,Update!$C$2:$D$115,2,FALSE),"")</f>
+        <f>IFERROR(VLOOKUP(A110,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>{0} 단계</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
-        <v>339</v>
+        <v>485</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>340</v>
+        <v>502</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>341</v>
+        <v>514</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>437</v>
+        <v>486</v>
       </c>
       <c r="G111" t="str">
-        <f>IFERROR(VLOOKUP(A111,Update!$C$2:$D$115,2,FALSE),"")</f>
-        <v>다음에만 적용: {0}</v>
+        <f>IFERROR(VLOOKUP(A111,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>특정 동물인 폰</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
-        <v>342</v>
+        <v>487</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>343</v>
+        <v>503</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>344</v>
+        <v>515</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>438</v>
+        <v>488</v>
       </c>
       <c r="G112" t="str">
-        <f>IFERROR(VLOOKUP(A112,Update!$C$2:$D$115,2,FALSE),"")</f>
-        <v>모든 상태</v>
+        <f>IFERROR(VLOOKUP(A112,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>특정 성별인 폰</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
-        <v>345</v>
+        <v>489</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>346</v>
+        <v>504</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>347</v>
+        <v>516</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>439</v>
+        <v>490</v>
       </c>
       <c r="G113" t="str">
-        <f>IFERROR(VLOOKUP(A113,Update!$C$2:$D$115,2,FALSE),"")</f>
-        <v>패시브 상태</v>
+        <f>IFERROR(VLOOKUP(A113,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>특정 나이대의 폰</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G114" t="str">
-        <f>IFERROR(VLOOKUP(A114,Update!$C$2:$D$115,2,FALSE),"")</f>
-        <v>공격적 상태</v>
+        <f>IFERROR(VLOOKUP(A114,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>다음에만 적용: {0}</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="G115" t="str">
+        <f>IFERROR(VLOOKUP(A115,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>모든 상태</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A116" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="G116" t="str">
+        <f>IFERROR(VLOOKUP(A116,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>패시브 상태</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A117" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G117" t="str">
+        <f>IFERROR(VLOOKUP(A117,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>공격적 상태</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A118" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C115" s="1" t="s">
+      <c r="B118" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="D115" s="1" t="s">
+      <c r="D118" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="G115" t="str">
-        <f>IFERROR(VLOOKUP(A115,Update!$C$2:$D$115,2,FALSE),"")</f>
+      <c r="G118" t="str">
+        <f>IFERROR(VLOOKUP(A118,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
         <v>이것은 재정의 규칙입니다. 현재 아이콘에 대한 조건이 충족되는 시간 동안에만 현재 아이콘을 재정의합니다.</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A119" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="G119" t="str">
+        <f>IFERROR(VLOOKUP(A119,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>규칙 복사</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A120" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="G120" t="str">
+        <f>IFERROR(VLOOKUP(A120,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>남성</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A121" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="G121" t="str">
+        <f>IFERROR(VLOOKUP(A121,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>여성</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A122" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="G122" t="str">
+        <f>IFERROR(VLOOKUP(A122,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>동물</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A123" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G123" t="str">
+        <f>IFERROR(VLOOKUP(A123,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>동물임</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A124" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="G124" t="str">
+        <f>IFERROR(VLOOKUP(A124,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>동물 아님</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A125" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="G125" t="str">
+        <f>IFERROR(VLOOKUP(A125,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>최소 나이 제한: {0}</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A126" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="G126" t="str">
+        <f>IFERROR(VLOOKUP(A126,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>최대 나이 제한: {0}</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A127" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="G127" t="str">
+        <f>IFERROR(VLOOKUP(A127,Update_231204!$C$2:$D$127,2,FALSE),"")</f>
+        <v>최대 나이 제한: 제한 없음</v>
       </c>
     </row>
   </sheetData>
@@ -4319,6 +4719,1538 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76EDFEB-7067-4F91-B123-2E6C05018DC7}">
+  <dimension ref="C2:E127"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E2">
+        <f>MATCH(C2,Sheet!$A$2:$A$127,0)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>355</v>
+      </c>
+      <c r="E3">
+        <f>MATCH(C3,Sheet!$A$2:$A$127,0)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" t="s">
+        <v>356</v>
+      </c>
+      <c r="E4">
+        <f>MATCH(C4,Sheet!$A$2:$A$127,0)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>357</v>
+      </c>
+      <c r="E5">
+        <f>MATCH(C5,Sheet!$A$2:$A$127,0)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>358</v>
+      </c>
+      <c r="E6">
+        <f>MATCH(C6,Sheet!$A$2:$A$127,0)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>359</v>
+      </c>
+      <c r="E7">
+        <f>MATCH(C7,Sheet!$A$2:$A$127,0)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>360</v>
+      </c>
+      <c r="E8">
+        <f>MATCH(C8,Sheet!$A$2:$A$127,0)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E9">
+        <f>MATCH(C9,Sheet!$A$2:$A$127,0)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>362</v>
+      </c>
+      <c r="E10">
+        <f>MATCH(C10,Sheet!$A$2:$A$127,0)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" t="s">
+        <v>363</v>
+      </c>
+      <c r="E11">
+        <f>MATCH(C11,Sheet!$A$2:$A$127,0)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" t="s">
+        <v>364</v>
+      </c>
+      <c r="E12">
+        <f>MATCH(C12,Sheet!$A$2:$A$127,0)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" t="s">
+        <v>365</v>
+      </c>
+      <c r="E13">
+        <f>MATCH(C13,Sheet!$A$2:$A$127,0)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" t="s">
+        <v>366</v>
+      </c>
+      <c r="E14">
+        <f>MATCH(C14,Sheet!$A$2:$A$127,0)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>367</v>
+      </c>
+      <c r="E15">
+        <f>MATCH(C15,Sheet!$A$2:$A$127,0)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D16" t="s">
+        <v>368</v>
+      </c>
+      <c r="E16">
+        <f>MATCH(C16,Sheet!$A$2:$A$127,0)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>369</v>
+      </c>
+      <c r="E17">
+        <f>MATCH(C17,Sheet!$A$2:$A$127,0)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" t="s">
+        <v>370</v>
+      </c>
+      <c r="E18">
+        <f>MATCH(C18,Sheet!$A$2:$A$127,0)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" t="s">
+        <v>371</v>
+      </c>
+      <c r="E19">
+        <f>MATCH(C19,Sheet!$A$2:$A$127,0)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" t="s">
+        <v>372</v>
+      </c>
+      <c r="E20">
+        <f>MATCH(C20,Sheet!$A$2:$A$127,0)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" t="s">
+        <v>373</v>
+      </c>
+      <c r="E21">
+        <f>MATCH(C21,Sheet!$A$2:$A$127,0)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s">
+        <v>374</v>
+      </c>
+      <c r="E22">
+        <f>MATCH(C22,Sheet!$A$2:$A$127,0)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" t="s">
+        <v>375</v>
+      </c>
+      <c r="E23">
+        <f>MATCH(C23,Sheet!$A$2:$A$127,0)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" t="s">
+        <v>376</v>
+      </c>
+      <c r="E24">
+        <f>MATCH(C24,Sheet!$A$2:$A$127,0)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C25" t="s">
+        <v>159</v>
+      </c>
+      <c r="D25" t="s">
+        <v>377</v>
+      </c>
+      <c r="E25">
+        <f>MATCH(C25,Sheet!$A$2:$A$127,0)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C26" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" t="s">
+        <v>378</v>
+      </c>
+      <c r="E26">
+        <f>MATCH(C26,Sheet!$A$2:$A$127,0)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C27" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" t="s">
+        <v>379</v>
+      </c>
+      <c r="E27">
+        <f>MATCH(C27,Sheet!$A$2:$A$127,0)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" t="s">
+        <v>380</v>
+      </c>
+      <c r="E28">
+        <f>MATCH(C28,Sheet!$A$2:$A$127,0)</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C29" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" t="s">
+        <v>381</v>
+      </c>
+      <c r="E29">
+        <f>MATCH(C29,Sheet!$A$2:$A$127,0)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" t="s">
+        <v>382</v>
+      </c>
+      <c r="E30">
+        <f>MATCH(C30,Sheet!$A$2:$A$127,0)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C31" t="s">
+        <v>177</v>
+      </c>
+      <c r="D31" t="s">
+        <v>383</v>
+      </c>
+      <c r="E31">
+        <f>MATCH(C31,Sheet!$A$2:$A$127,0)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C32" t="s">
+        <v>180</v>
+      </c>
+      <c r="D32" t="s">
+        <v>384</v>
+      </c>
+      <c r="E32">
+        <f>MATCH(C32,Sheet!$A$2:$A$127,0)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
+        <v>183</v>
+      </c>
+      <c r="D33" t="s">
+        <v>385</v>
+      </c>
+      <c r="E33">
+        <f>MATCH(C33,Sheet!$A$2:$A$127,0)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C34" t="s">
+        <v>186</v>
+      </c>
+      <c r="D34" t="s">
+        <v>386</v>
+      </c>
+      <c r="E34">
+        <f>MATCH(C34,Sheet!$A$2:$A$127,0)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C35" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" t="s">
+        <v>387</v>
+      </c>
+      <c r="E35">
+        <f>MATCH(C35,Sheet!$A$2:$A$127,0)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C36" t="s">
+        <v>192</v>
+      </c>
+      <c r="D36" t="s">
+        <v>388</v>
+      </c>
+      <c r="E36">
+        <f>MATCH(C36,Sheet!$A$2:$A$127,0)</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C37" t="s">
+        <v>195</v>
+      </c>
+      <c r="D37" t="s">
+        <v>389</v>
+      </c>
+      <c r="E37">
+        <f>MATCH(C37,Sheet!$A$2:$A$127,0)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C38" t="s">
+        <v>198</v>
+      </c>
+      <c r="D38" t="s">
+        <v>390</v>
+      </c>
+      <c r="E38">
+        <f>MATCH(C38,Sheet!$A$2:$A$127,0)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C39" t="s">
+        <v>201</v>
+      </c>
+      <c r="D39" t="s">
+        <v>391</v>
+      </c>
+      <c r="E39">
+        <f>MATCH(C39,Sheet!$A$2:$A$127,0)</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C40" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" t="s">
+        <v>392</v>
+      </c>
+      <c r="E40">
+        <f>MATCH(C40,Sheet!$A$2:$A$127,0)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C41" t="s">
+        <v>207</v>
+      </c>
+      <c r="D41" t="s">
+        <v>393</v>
+      </c>
+      <c r="E41">
+        <f>MATCH(C41,Sheet!$A$2:$A$127,0)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C42" t="s">
+        <v>210</v>
+      </c>
+      <c r="D42" t="s">
+        <v>394</v>
+      </c>
+      <c r="E42">
+        <f>MATCH(C42,Sheet!$A$2:$A$127,0)</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C43" t="s">
+        <v>213</v>
+      </c>
+      <c r="D43" t="s">
+        <v>395</v>
+      </c>
+      <c r="E43">
+        <f>MATCH(C43,Sheet!$A$2:$A$127,0)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C44" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44" t="s">
+        <v>396</v>
+      </c>
+      <c r="E44">
+        <f>MATCH(C44,Sheet!$A$2:$A$127,0)</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C45" t="s">
+        <v>219</v>
+      </c>
+      <c r="D45" t="s">
+        <v>397</v>
+      </c>
+      <c r="E45">
+        <f>MATCH(C45,Sheet!$A$2:$A$127,0)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C46" t="s">
+        <v>222</v>
+      </c>
+      <c r="D46" t="s">
+        <v>398</v>
+      </c>
+      <c r="E46">
+        <f>MATCH(C46,Sheet!$A$2:$A$127,0)</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C47" t="s">
+        <v>225</v>
+      </c>
+      <c r="D47" t="s">
+        <v>399</v>
+      </c>
+      <c r="E47">
+        <f>MATCH(C47,Sheet!$A$2:$A$127,0)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C48" t="s">
+        <v>228</v>
+      </c>
+      <c r="D48" t="s">
+        <v>400</v>
+      </c>
+      <c r="E48">
+        <f>MATCH(C48,Sheet!$A$2:$A$127,0)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C49" t="s">
+        <v>231</v>
+      </c>
+      <c r="D49" t="s">
+        <v>401</v>
+      </c>
+      <c r="E49">
+        <f>MATCH(C49,Sheet!$A$2:$A$127,0)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C50" t="s">
+        <v>234</v>
+      </c>
+      <c r="D50" t="s">
+        <v>402</v>
+      </c>
+      <c r="E50">
+        <f>MATCH(C50,Sheet!$A$2:$A$127,0)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C51" t="s">
+        <v>237</v>
+      </c>
+      <c r="D51" t="s">
+        <v>403</v>
+      </c>
+      <c r="E51">
+        <f>MATCH(C51,Sheet!$A$2:$A$127,0)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C52" t="s">
+        <v>240</v>
+      </c>
+      <c r="D52" t="s">
+        <v>404</v>
+      </c>
+      <c r="E52">
+        <f>MATCH(C52,Sheet!$A$2:$A$127,0)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C53" t="s">
+        <v>246</v>
+      </c>
+      <c r="D53" t="s">
+        <v>405</v>
+      </c>
+      <c r="E53">
+        <f>MATCH(C53,Sheet!$A$2:$A$127,0)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C54" t="s">
+        <v>249</v>
+      </c>
+      <c r="D54" t="s">
+        <v>406</v>
+      </c>
+      <c r="E54">
+        <f>MATCH(C54,Sheet!$A$2:$A$127,0)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C55" t="s">
+        <v>252</v>
+      </c>
+      <c r="D55" t="s">
+        <v>407</v>
+      </c>
+      <c r="E55">
+        <f>MATCH(C55,Sheet!$A$2:$A$127,0)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C56" t="s">
+        <v>255</v>
+      </c>
+      <c r="D56" t="s">
+        <v>408</v>
+      </c>
+      <c r="E56">
+        <f>MATCH(C56,Sheet!$A$2:$A$127,0)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C57" t="s">
+        <v>258</v>
+      </c>
+      <c r="D57" t="s">
+        <v>409</v>
+      </c>
+      <c r="E57">
+        <f>MATCH(C57,Sheet!$A$2:$A$127,0)</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C58" t="s">
+        <v>261</v>
+      </c>
+      <c r="D58" t="s">
+        <v>410</v>
+      </c>
+      <c r="E58">
+        <f>MATCH(C58,Sheet!$A$2:$A$127,0)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C59" t="s">
+        <v>264</v>
+      </c>
+      <c r="D59" t="s">
+        <v>411</v>
+      </c>
+      <c r="E59">
+        <f>MATCH(C59,Sheet!$A$2:$A$127,0)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C60" t="s">
+        <v>267</v>
+      </c>
+      <c r="D60" t="s">
+        <v>412</v>
+      </c>
+      <c r="E60">
+        <f>MATCH(C60,Sheet!$A$2:$A$127,0)</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C61" t="s">
+        <v>270</v>
+      </c>
+      <c r="D61" t="s">
+        <v>413</v>
+      </c>
+      <c r="E61">
+        <f>MATCH(C61,Sheet!$A$2:$A$127,0)</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C62" t="s">
+        <v>273</v>
+      </c>
+      <c r="D62" t="s">
+        <v>414</v>
+      </c>
+      <c r="E62">
+        <f>MATCH(C62,Sheet!$A$2:$A$127,0)</f>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C63" t="s">
+        <v>276</v>
+      </c>
+      <c r="D63" t="s">
+        <v>415</v>
+      </c>
+      <c r="E63">
+        <f>MATCH(C63,Sheet!$A$2:$A$127,0)</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C64" t="s">
+        <v>279</v>
+      </c>
+      <c r="D64" t="s">
+        <v>416</v>
+      </c>
+      <c r="E64">
+        <f>MATCH(C64,Sheet!$A$2:$A$127,0)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C65" t="s">
+        <v>282</v>
+      </c>
+      <c r="D65" t="s">
+        <v>417</v>
+      </c>
+      <c r="E65">
+        <f>MATCH(C65,Sheet!$A$2:$A$127,0)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C66" t="s">
+        <v>285</v>
+      </c>
+      <c r="D66" t="s">
+        <v>418</v>
+      </c>
+      <c r="E66">
+        <f>MATCH(C66,Sheet!$A$2:$A$127,0)</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C67" t="s">
+        <v>288</v>
+      </c>
+      <c r="D67" t="s">
+        <v>419</v>
+      </c>
+      <c r="E67">
+        <f>MATCH(C67,Sheet!$A$2:$A$127,0)</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C68" t="s">
+        <v>291</v>
+      </c>
+      <c r="D68" t="s">
+        <v>420</v>
+      </c>
+      <c r="E68">
+        <f>MATCH(C68,Sheet!$A$2:$A$127,0)</f>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C69" t="s">
+        <v>294</v>
+      </c>
+      <c r="D69" t="s">
+        <v>421</v>
+      </c>
+      <c r="E69">
+        <f>MATCH(C69,Sheet!$A$2:$A$127,0)</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C70" t="s">
+        <v>297</v>
+      </c>
+      <c r="D70" t="s">
+        <v>422</v>
+      </c>
+      <c r="E70">
+        <f>MATCH(C70,Sheet!$A$2:$A$127,0)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C71" t="s">
+        <v>300</v>
+      </c>
+      <c r="D71" t="s">
+        <v>423</v>
+      </c>
+      <c r="E71">
+        <f>MATCH(C71,Sheet!$A$2:$A$127,0)</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C72" t="s">
+        <v>306</v>
+      </c>
+      <c r="D72" t="s">
+        <v>424</v>
+      </c>
+      <c r="E72">
+        <f>MATCH(C72,Sheet!$A$2:$A$127,0)</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C73" t="s">
+        <v>309</v>
+      </c>
+      <c r="D73" t="s">
+        <v>425</v>
+      </c>
+      <c r="E73">
+        <f>MATCH(C73,Sheet!$A$2:$A$127,0)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C74" t="s">
+        <v>312</v>
+      </c>
+      <c r="D74" t="s">
+        <v>426</v>
+      </c>
+      <c r="E74">
+        <f>MATCH(C74,Sheet!$A$2:$A$127,0)</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C75" t="s">
+        <v>315</v>
+      </c>
+      <c r="D75" t="s">
+        <v>427</v>
+      </c>
+      <c r="E75">
+        <f>MATCH(C75,Sheet!$A$2:$A$127,0)</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C76" t="s">
+        <v>318</v>
+      </c>
+      <c r="D76" t="s">
+        <v>428</v>
+      </c>
+      <c r="E76">
+        <f>MATCH(C76,Sheet!$A$2:$A$127,0)</f>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C77" t="s">
+        <v>321</v>
+      </c>
+      <c r="D77" t="s">
+        <v>429</v>
+      </c>
+      <c r="E77">
+        <f>MATCH(C77,Sheet!$A$2:$A$127,0)</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="78" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C78" t="s">
+        <v>243</v>
+      </c>
+      <c r="D78" t="s">
+        <v>430</v>
+      </c>
+      <c r="E78">
+        <f>MATCH(C78,Sheet!$A$2:$A$127,0)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C79" t="s">
+        <v>303</v>
+      </c>
+      <c r="D79" t="s">
+        <v>431</v>
+      </c>
+      <c r="E79">
+        <f>MATCH(C79,Sheet!$A$2:$A$127,0)</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C80" t="s">
+        <v>324</v>
+      </c>
+      <c r="D80" t="s">
+        <v>432</v>
+      </c>
+      <c r="E80">
+        <f>MATCH(C80,Sheet!$A$2:$A$127,0)</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C81" t="s">
+        <v>327</v>
+      </c>
+      <c r="D81" t="s">
+        <v>433</v>
+      </c>
+      <c r="E81">
+        <f>MATCH(C81,Sheet!$A$2:$A$127,0)</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C82" t="s">
+        <v>330</v>
+      </c>
+      <c r="D82" t="s">
+        <v>434</v>
+      </c>
+      <c r="E82">
+        <f>MATCH(C82,Sheet!$A$2:$A$127,0)</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C83" t="s">
+        <v>333</v>
+      </c>
+      <c r="D83" t="s">
+        <v>435</v>
+      </c>
+      <c r="E83">
+        <f>MATCH(C83,Sheet!$A$2:$A$127,0)</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C84" t="s">
+        <v>336</v>
+      </c>
+      <c r="D84" t="s">
+        <v>436</v>
+      </c>
+      <c r="E84">
+        <f>MATCH(C84,Sheet!$A$2:$A$127,0)</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C85" t="s">
+        <v>339</v>
+      </c>
+      <c r="D85" t="s">
+        <v>437</v>
+      </c>
+      <c r="E85">
+        <f>MATCH(C85,Sheet!$A$2:$A$127,0)</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C86" t="s">
+        <v>342</v>
+      </c>
+      <c r="D86" t="s">
+        <v>438</v>
+      </c>
+      <c r="E86">
+        <f>MATCH(C86,Sheet!$A$2:$A$127,0)</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C87" t="s">
+        <v>345</v>
+      </c>
+      <c r="D87" t="s">
+        <v>439</v>
+      </c>
+      <c r="E87">
+        <f>MATCH(C87,Sheet!$A$2:$A$127,0)</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C88" t="s">
+        <v>348</v>
+      </c>
+      <c r="D88" t="s">
+        <v>440</v>
+      </c>
+      <c r="E88">
+        <f>MATCH(C88,Sheet!$A$2:$A$127,0)</f>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C89" t="s">
+        <v>351</v>
+      </c>
+      <c r="D89" t="s">
+        <v>441</v>
+      </c>
+      <c r="E89">
+        <f>MATCH(C89,Sheet!$A$2:$A$127,0)</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C90" t="s">
+        <v>467</v>
+      </c>
+      <c r="D90" t="s">
+        <v>468</v>
+      </c>
+      <c r="E90">
+        <f>MATCH(C90,Sheet!$A$2:$A$127,0)</f>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C91" t="s">
+        <v>469</v>
+      </c>
+      <c r="D91" t="s">
+        <v>470</v>
+      </c>
+      <c r="E91">
+        <f>MATCH(C91,Sheet!$A$2:$A$127,0)</f>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C92" t="s">
+        <v>471</v>
+      </c>
+      <c r="D92" t="s">
+        <v>472</v>
+      </c>
+      <c r="E92">
+        <f>MATCH(C92,Sheet!$A$2:$A$127,0)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C93" t="s">
+        <v>473</v>
+      </c>
+      <c r="D93" t="s">
+        <v>474</v>
+      </c>
+      <c r="E93">
+        <f>MATCH(C93,Sheet!$A$2:$A$127,0)</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C94" t="s">
+        <v>475</v>
+      </c>
+      <c r="D94" t="s">
+        <v>476</v>
+      </c>
+      <c r="E94">
+        <f>MATCH(C94,Sheet!$A$2:$A$127,0)</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C95" t="s">
+        <v>477</v>
+      </c>
+      <c r="D95" t="s">
+        <v>478</v>
+      </c>
+      <c r="E95">
+        <f>MATCH(C95,Sheet!$A$2:$A$127,0)</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C96" t="s">
+        <v>479</v>
+      </c>
+      <c r="D96" t="s">
+        <v>480</v>
+      </c>
+      <c r="E96">
+        <f>MATCH(C96,Sheet!$A$2:$A$127,0)</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C97" t="s">
+        <v>481</v>
+      </c>
+      <c r="D97" t="s">
+        <v>482</v>
+      </c>
+      <c r="E97">
+        <f>MATCH(C97,Sheet!$A$2:$A$127,0)</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="98" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C98" t="s">
+        <v>483</v>
+      </c>
+      <c r="D98" t="s">
+        <v>484</v>
+      </c>
+      <c r="E98">
+        <f>MATCH(C98,Sheet!$A$2:$A$127,0)</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C99" t="s">
+        <v>485</v>
+      </c>
+      <c r="D99" t="s">
+        <v>486</v>
+      </c>
+      <c r="E99">
+        <f>MATCH(C99,Sheet!$A$2:$A$127,0)</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="100" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C100" t="s">
+        <v>487</v>
+      </c>
+      <c r="D100" t="s">
+        <v>488</v>
+      </c>
+      <c r="E100">
+        <f>MATCH(C100,Sheet!$A$2:$A$127,0)</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="101" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C101" t="s">
+        <v>489</v>
+      </c>
+      <c r="D101" t="s">
+        <v>490</v>
+      </c>
+      <c r="E101">
+        <f>MATCH(C101,Sheet!$A$2:$A$127,0)</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C102" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" t="s">
+        <v>442</v>
+      </c>
+      <c r="E102">
+        <f>MATCH(C102,Sheet!$A$2:$A$127,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C103" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" t="s">
+        <v>443</v>
+      </c>
+      <c r="E103">
+        <f>MATCH(C103,Sheet!$A$2:$A$127,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C104" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104" t="s">
+        <v>444</v>
+      </c>
+      <c r="E104">
+        <f>MATCH(C104,Sheet!$A$2:$A$127,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C105" t="s">
+        <v>19</v>
+      </c>
+      <c r="D105" t="s">
+        <v>445</v>
+      </c>
+      <c r="E105">
+        <f>MATCH(C105,Sheet!$A$2:$A$127,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C106" t="s">
+        <v>23</v>
+      </c>
+      <c r="D106" t="s">
+        <v>446</v>
+      </c>
+      <c r="E106">
+        <f>MATCH(C106,Sheet!$A$2:$A$127,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C107" t="s">
+        <v>26</v>
+      </c>
+      <c r="D107" t="s">
+        <v>447</v>
+      </c>
+      <c r="E107">
+        <f>MATCH(C107,Sheet!$A$2:$A$127,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C108" t="s">
+        <v>29</v>
+      </c>
+      <c r="D108" t="s">
+        <v>448</v>
+      </c>
+      <c r="E108">
+        <f>MATCH(C108,Sheet!$A$2:$A$127,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C109" t="s">
+        <v>32</v>
+      </c>
+      <c r="D109" t="s">
+        <v>491</v>
+      </c>
+      <c r="E109">
+        <f>MATCH(C109,Sheet!$A$2:$A$127,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C110" t="s">
+        <v>35</v>
+      </c>
+      <c r="D110" t="s">
+        <v>450</v>
+      </c>
+      <c r="E110">
+        <f>MATCH(C110,Sheet!$A$2:$A$127,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="111" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C111" t="s">
+        <v>38</v>
+      </c>
+      <c r="D111" t="s">
+        <v>451</v>
+      </c>
+      <c r="E111">
+        <f>MATCH(C111,Sheet!$A$2:$A$127,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C112" t="s">
+        <v>41</v>
+      </c>
+      <c r="D112" t="s">
+        <v>43</v>
+      </c>
+      <c r="E112">
+        <f>MATCH(C112,Sheet!$A$2:$A$127,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C113" t="s">
+        <v>44</v>
+      </c>
+      <c r="D113" t="s">
+        <v>452</v>
+      </c>
+      <c r="E113">
+        <f>MATCH(C113,Sheet!$A$2:$A$127,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C114" t="s">
+        <v>47</v>
+      </c>
+      <c r="D114" t="s">
+        <v>49</v>
+      </c>
+      <c r="E114">
+        <f>MATCH(C114,Sheet!$A$2:$A$127,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="115" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C115" t="s">
+        <v>50</v>
+      </c>
+      <c r="D115" t="s">
+        <v>453</v>
+      </c>
+      <c r="E115">
+        <f>MATCH(C115,Sheet!$A$2:$A$127,0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C116" t="s">
+        <v>53</v>
+      </c>
+      <c r="D116" t="s">
+        <v>55</v>
+      </c>
+      <c r="E116">
+        <f>MATCH(C116,Sheet!$A$2:$A$127,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C117" t="s">
+        <v>56</v>
+      </c>
+      <c r="D117" t="s">
+        <v>454</v>
+      </c>
+      <c r="E117">
+        <f>MATCH(C117,Sheet!$A$2:$A$127,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C118" t="s">
+        <v>65</v>
+      </c>
+      <c r="D118" t="s">
+        <v>455</v>
+      </c>
+      <c r="E118">
+        <f>MATCH(C118,Sheet!$A$2:$A$127,0)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="119" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C119" t="s">
+        <v>68</v>
+      </c>
+      <c r="D119" t="s">
+        <v>456</v>
+      </c>
+      <c r="E119">
+        <f>MATCH(C119,Sheet!$A$2:$A$127,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C120" t="s">
+        <v>71</v>
+      </c>
+      <c r="D120" t="s">
+        <v>457</v>
+      </c>
+      <c r="E120">
+        <f>MATCH(C120,Sheet!$A$2:$A$127,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="121" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C121" t="s">
+        <v>74</v>
+      </c>
+      <c r="D121" t="s">
+        <v>458</v>
+      </c>
+      <c r="E121">
+        <f>MATCH(C121,Sheet!$A$2:$A$127,0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="122" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C122" t="s">
+        <v>83</v>
+      </c>
+      <c r="D122" t="s">
+        <v>459</v>
+      </c>
+      <c r="E122">
+        <f>MATCH(C122,Sheet!$A$2:$A$127,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="123" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C123" t="s">
+        <v>86</v>
+      </c>
+      <c r="D123" t="s">
+        <v>460</v>
+      </c>
+      <c r="E123">
+        <f>MATCH(C123,Sheet!$A$2:$A$127,0)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C124" t="s">
+        <v>59</v>
+      </c>
+      <c r="D124" t="s">
+        <v>61</v>
+      </c>
+      <c r="E124">
+        <f>MATCH(C124,Sheet!$A$2:$A$127,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C125" t="s">
+        <v>62</v>
+      </c>
+      <c r="D125" t="s">
+        <v>461</v>
+      </c>
+      <c r="E125">
+        <f>MATCH(C125,Sheet!$A$2:$A$127,0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="126" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C126" t="s">
+        <v>77</v>
+      </c>
+      <c r="D126" t="s">
+        <v>462</v>
+      </c>
+      <c r="E126">
+        <f>MATCH(C126,Sheet!$A$2:$A$127,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" spans="3:5" x14ac:dyDescent="0.45">
+      <c r="C127" t="s">
+        <v>80</v>
+      </c>
+      <c r="D127" t="s">
+        <v>463</v>
+      </c>
+      <c r="E127">
+        <f>MATCH(C127,Sheet!$A$2:$A$127,0)</f>
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790944B4-905C-45E5-9E79-51B5614D9AF8}">
   <dimension ref="A1:E115"/>
   <sheetViews>
@@ -4357,7 +6289,7 @@
         <v>354</v>
       </c>
       <c r="E2">
-        <f>IF(ISERROR(B2),"",MATCH(C2,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B2),"",MATCH(C2,Sheet!$A$2:$A$118,0))</f>
         <v>27</v>
       </c>
     </row>
@@ -4373,7 +6305,7 @@
         <v>355</v>
       </c>
       <c r="E3">
-        <f>IF(ISERROR(B3),"",MATCH(C3,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B3),"",MATCH(C3,Sheet!$A$2:$A$118,0))</f>
         <v>28</v>
       </c>
     </row>
@@ -4389,7 +6321,7 @@
         <v>356</v>
       </c>
       <c r="E4">
-        <f>IF(ISERROR(B4),"",MATCH(C4,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B4),"",MATCH(C4,Sheet!$A$2:$A$118,0))</f>
         <v>29</v>
       </c>
     </row>
@@ -4405,7 +6337,7 @@
         <v>357</v>
       </c>
       <c r="E5">
-        <f>IF(ISERROR(B5),"",MATCH(C5,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B5),"",MATCH(C5,Sheet!$A$2:$A$118,0))</f>
         <v>30</v>
       </c>
     </row>
@@ -4421,7 +6353,7 @@
         <v>358</v>
       </c>
       <c r="E6">
-        <f>IF(ISERROR(B6),"",MATCH(C6,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B6),"",MATCH(C6,Sheet!$A$2:$A$118,0))</f>
         <v>31</v>
       </c>
     </row>
@@ -4437,7 +6369,7 @@
         <v>359</v>
       </c>
       <c r="E7">
-        <f>IF(ISERROR(B7),"",MATCH(C7,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B7),"",MATCH(C7,Sheet!$A$2:$A$118,0))</f>
         <v>32</v>
       </c>
     </row>
@@ -4453,7 +6385,7 @@
         <v>360</v>
       </c>
       <c r="E8">
-        <f>IF(ISERROR(B8),"",MATCH(C8,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B8),"",MATCH(C8,Sheet!$A$2:$A$118,0))</f>
         <v>33</v>
       </c>
     </row>
@@ -4469,7 +6401,7 @@
         <v>361</v>
       </c>
       <c r="E9">
-        <f>IF(ISERROR(B9),"",MATCH(C9,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B9),"",MATCH(C9,Sheet!$A$2:$A$118,0))</f>
         <v>34</v>
       </c>
     </row>
@@ -4485,7 +6417,7 @@
         <v>362</v>
       </c>
       <c r="E10">
-        <f>IF(ISERROR(B10),"",MATCH(C10,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B10),"",MATCH(C10,Sheet!$A$2:$A$118,0))</f>
         <v>35</v>
       </c>
     </row>
@@ -4501,7 +6433,7 @@
         <v>363</v>
       </c>
       <c r="E11">
-        <f>IF(ISERROR(B11),"",MATCH(C11,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B11),"",MATCH(C11,Sheet!$A$2:$A$118,0))</f>
         <v>36</v>
       </c>
     </row>
@@ -4517,7 +6449,7 @@
         <v>364</v>
       </c>
       <c r="E12">
-        <f>IF(ISERROR(B12),"",MATCH(C12,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B12),"",MATCH(C12,Sheet!$A$2:$A$118,0))</f>
         <v>37</v>
       </c>
     </row>
@@ -4533,7 +6465,7 @@
         <v>365</v>
       </c>
       <c r="E13">
-        <f>IF(ISERROR(B13),"",MATCH(C13,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B13),"",MATCH(C13,Sheet!$A$2:$A$118,0))</f>
         <v>38</v>
       </c>
     </row>
@@ -4549,7 +6481,7 @@
         <v>366</v>
       </c>
       <c r="E14">
-        <f>IF(ISERROR(B14),"",MATCH(C14,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B14),"",MATCH(C14,Sheet!$A$2:$A$118,0))</f>
         <v>39</v>
       </c>
     </row>
@@ -4565,7 +6497,7 @@
         <v>367</v>
       </c>
       <c r="E15">
-        <f>IF(ISERROR(B15),"",MATCH(C15,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B15),"",MATCH(C15,Sheet!$A$2:$A$118,0))</f>
         <v>40</v>
       </c>
     </row>
@@ -4581,7 +6513,7 @@
         <v>368</v>
       </c>
       <c r="E16">
-        <f>IF(ISERROR(B16),"",MATCH(C16,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B16),"",MATCH(C16,Sheet!$A$2:$A$118,0))</f>
         <v>41</v>
       </c>
     </row>
@@ -4597,7 +6529,7 @@
         <v>369</v>
       </c>
       <c r="E17">
-        <f>IF(ISERROR(B17),"",MATCH(C17,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B17),"",MATCH(C17,Sheet!$A$2:$A$118,0))</f>
         <v>42</v>
       </c>
     </row>
@@ -4613,7 +6545,7 @@
         <v>370</v>
       </c>
       <c r="E18">
-        <f>IF(ISERROR(B18),"",MATCH(C18,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B18),"",MATCH(C18,Sheet!$A$2:$A$118,0))</f>
         <v>43</v>
       </c>
     </row>
@@ -4629,7 +6561,7 @@
         <v>371</v>
       </c>
       <c r="E19">
-        <f>IF(ISERROR(B19),"",MATCH(C19,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B19),"",MATCH(C19,Sheet!$A$2:$A$118,0))</f>
         <v>44</v>
       </c>
     </row>
@@ -4645,7 +6577,7 @@
         <v>372</v>
       </c>
       <c r="E20">
-        <f>IF(ISERROR(B20),"",MATCH(C20,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B20),"",MATCH(C20,Sheet!$A$2:$A$118,0))</f>
         <v>45</v>
       </c>
     </row>
@@ -4661,7 +6593,7 @@
         <v>373</v>
       </c>
       <c r="E21">
-        <f>IF(ISERROR(B21),"",MATCH(C21,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B21),"",MATCH(C21,Sheet!$A$2:$A$118,0))</f>
         <v>46</v>
       </c>
     </row>
@@ -4677,7 +6609,7 @@
         <v>374</v>
       </c>
       <c r="E22">
-        <f>IF(ISERROR(B22),"",MATCH(C22,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B22),"",MATCH(C22,Sheet!$A$2:$A$118,0))</f>
         <v>47</v>
       </c>
     </row>
@@ -4693,7 +6625,7 @@
         <v>375</v>
       </c>
       <c r="E23">
-        <f>IF(ISERROR(B23),"",MATCH(C23,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B23),"",MATCH(C23,Sheet!$A$2:$A$118,0))</f>
         <v>48</v>
       </c>
     </row>
@@ -4709,7 +6641,7 @@
         <v>376</v>
       </c>
       <c r="E24">
-        <f>IF(ISERROR(B24),"",MATCH(C24,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B24),"",MATCH(C24,Sheet!$A$2:$A$118,0))</f>
         <v>49</v>
       </c>
     </row>
@@ -4725,7 +6657,7 @@
         <v>377</v>
       </c>
       <c r="E25">
-        <f>IF(ISERROR(B25),"",MATCH(C25,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B25),"",MATCH(C25,Sheet!$A$2:$A$118,0))</f>
         <v>50</v>
       </c>
     </row>
@@ -4741,7 +6673,7 @@
         <v>378</v>
       </c>
       <c r="E26">
-        <f>IF(ISERROR(B26),"",MATCH(C26,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B26),"",MATCH(C26,Sheet!$A$2:$A$118,0))</f>
         <v>51</v>
       </c>
     </row>
@@ -4757,7 +6689,7 @@
         <v>379</v>
       </c>
       <c r="E27">
-        <f>IF(ISERROR(B27),"",MATCH(C27,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B27),"",MATCH(C27,Sheet!$A$2:$A$118,0))</f>
         <v>52</v>
       </c>
     </row>
@@ -4773,7 +6705,7 @@
         <v>380</v>
       </c>
       <c r="E28">
-        <f>IF(ISERROR(B28),"",MATCH(C28,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B28),"",MATCH(C28,Sheet!$A$2:$A$118,0))</f>
         <v>53</v>
       </c>
     </row>
@@ -4789,7 +6721,7 @@
         <v>381</v>
       </c>
       <c r="E29">
-        <f>IF(ISERROR(B29),"",MATCH(C29,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B29),"",MATCH(C29,Sheet!$A$2:$A$118,0))</f>
         <v>54</v>
       </c>
     </row>
@@ -4805,7 +6737,7 @@
         <v>382</v>
       </c>
       <c r="E30">
-        <f>IF(ISERROR(B30),"",MATCH(C30,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B30),"",MATCH(C30,Sheet!$A$2:$A$118,0))</f>
         <v>55</v>
       </c>
     </row>
@@ -4821,7 +6753,7 @@
         <v>383</v>
       </c>
       <c r="E31">
-        <f>IF(ISERROR(B31),"",MATCH(C31,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B31),"",MATCH(C31,Sheet!$A$2:$A$118,0))</f>
         <v>56</v>
       </c>
     </row>
@@ -4837,7 +6769,7 @@
         <v>384</v>
       </c>
       <c r="E32">
-        <f>IF(ISERROR(B32),"",MATCH(C32,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B32),"",MATCH(C32,Sheet!$A$2:$A$118,0))</f>
         <v>57</v>
       </c>
     </row>
@@ -4853,7 +6785,7 @@
         <v>385</v>
       </c>
       <c r="E33">
-        <f>IF(ISERROR(B33),"",MATCH(C33,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B33),"",MATCH(C33,Sheet!$A$2:$A$118,0))</f>
         <v>58</v>
       </c>
     </row>
@@ -4869,7 +6801,7 @@
         <v>386</v>
       </c>
       <c r="E34">
-        <f>IF(ISERROR(B34),"",MATCH(C34,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B34),"",MATCH(C34,Sheet!$A$2:$A$118,0))</f>
         <v>59</v>
       </c>
     </row>
@@ -4885,7 +6817,7 @@
         <v>387</v>
       </c>
       <c r="E35">
-        <f>IF(ISERROR(B35),"",MATCH(C35,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B35),"",MATCH(C35,Sheet!$A$2:$A$118,0))</f>
         <v>60</v>
       </c>
     </row>
@@ -4901,7 +6833,7 @@
         <v>388</v>
       </c>
       <c r="E36">
-        <f>IF(ISERROR(B36),"",MATCH(C36,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B36),"",MATCH(C36,Sheet!$A$2:$A$118,0))</f>
         <v>61</v>
       </c>
     </row>
@@ -4917,7 +6849,7 @@
         <v>389</v>
       </c>
       <c r="E37">
-        <f>IF(ISERROR(B37),"",MATCH(C37,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B37),"",MATCH(C37,Sheet!$A$2:$A$118,0))</f>
         <v>62</v>
       </c>
     </row>
@@ -4933,7 +6865,7 @@
         <v>390</v>
       </c>
       <c r="E38">
-        <f>IF(ISERROR(B38),"",MATCH(C38,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B38),"",MATCH(C38,Sheet!$A$2:$A$118,0))</f>
         <v>63</v>
       </c>
     </row>
@@ -4949,7 +6881,7 @@
         <v>391</v>
       </c>
       <c r="E39">
-        <f>IF(ISERROR(B39),"",MATCH(C39,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B39),"",MATCH(C39,Sheet!$A$2:$A$118,0))</f>
         <v>64</v>
       </c>
     </row>
@@ -4965,7 +6897,7 @@
         <v>392</v>
       </c>
       <c r="E40">
-        <f>IF(ISERROR(B40),"",MATCH(C40,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B40),"",MATCH(C40,Sheet!$A$2:$A$118,0))</f>
         <v>65</v>
       </c>
     </row>
@@ -4981,7 +6913,7 @@
         <v>393</v>
       </c>
       <c r="E41">
-        <f>IF(ISERROR(B41),"",MATCH(C41,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B41),"",MATCH(C41,Sheet!$A$2:$A$118,0))</f>
         <v>66</v>
       </c>
     </row>
@@ -4997,7 +6929,7 @@
         <v>394</v>
       </c>
       <c r="E42">
-        <f>IF(ISERROR(B42),"",MATCH(C42,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B42),"",MATCH(C42,Sheet!$A$2:$A$118,0))</f>
         <v>67</v>
       </c>
     </row>
@@ -5013,7 +6945,7 @@
         <v>395</v>
       </c>
       <c r="E43">
-        <f>IF(ISERROR(B43),"",MATCH(C43,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B43),"",MATCH(C43,Sheet!$A$2:$A$118,0))</f>
         <v>68</v>
       </c>
     </row>
@@ -5029,7 +6961,7 @@
         <v>396</v>
       </c>
       <c r="E44">
-        <f>IF(ISERROR(B44),"",MATCH(C44,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B44),"",MATCH(C44,Sheet!$A$2:$A$118,0))</f>
         <v>69</v>
       </c>
     </row>
@@ -5045,7 +6977,7 @@
         <v>397</v>
       </c>
       <c r="E45">
-        <f>IF(ISERROR(B45),"",MATCH(C45,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B45),"",MATCH(C45,Sheet!$A$2:$A$118,0))</f>
         <v>70</v>
       </c>
     </row>
@@ -5061,7 +6993,7 @@
         <v>398</v>
       </c>
       <c r="E46">
-        <f>IF(ISERROR(B46),"",MATCH(C46,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B46),"",MATCH(C46,Sheet!$A$2:$A$118,0))</f>
         <v>71</v>
       </c>
     </row>
@@ -5077,7 +7009,7 @@
         <v>399</v>
       </c>
       <c r="E47">
-        <f>IF(ISERROR(B47),"",MATCH(C47,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B47),"",MATCH(C47,Sheet!$A$2:$A$118,0))</f>
         <v>72</v>
       </c>
     </row>
@@ -5093,7 +7025,7 @@
         <v>400</v>
       </c>
       <c r="E48">
-        <f>IF(ISERROR(B48),"",MATCH(C48,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B48),"",MATCH(C48,Sheet!$A$2:$A$118,0))</f>
         <v>73</v>
       </c>
     </row>
@@ -5109,7 +7041,7 @@
         <v>401</v>
       </c>
       <c r="E49">
-        <f>IF(ISERROR(B49),"",MATCH(C49,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B49),"",MATCH(C49,Sheet!$A$2:$A$118,0))</f>
         <v>74</v>
       </c>
     </row>
@@ -5125,7 +7057,7 @@
         <v>402</v>
       </c>
       <c r="E50">
-        <f>IF(ISERROR(B50),"",MATCH(C50,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B50),"",MATCH(C50,Sheet!$A$2:$A$118,0))</f>
         <v>75</v>
       </c>
     </row>
@@ -5141,7 +7073,7 @@
         <v>403</v>
       </c>
       <c r="E51">
-        <f>IF(ISERROR(B51),"",MATCH(C51,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B51),"",MATCH(C51,Sheet!$A$2:$A$118,0))</f>
         <v>76</v>
       </c>
     </row>
@@ -5157,7 +7089,7 @@
         <v>404</v>
       </c>
       <c r="E52">
-        <f>IF(ISERROR(B52),"",MATCH(C52,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B52),"",MATCH(C52,Sheet!$A$2:$A$118,0))</f>
         <v>77</v>
       </c>
     </row>
@@ -5173,7 +7105,7 @@
         <v>405</v>
       </c>
       <c r="E53">
-        <f>IF(ISERROR(B53),"",MATCH(C53,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B53),"",MATCH(C53,Sheet!$A$2:$A$118,0))</f>
         <v>79</v>
       </c>
     </row>
@@ -5189,7 +7121,7 @@
         <v>406</v>
       </c>
       <c r="E54">
-        <f>IF(ISERROR(B54),"",MATCH(C54,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B54),"",MATCH(C54,Sheet!$A$2:$A$118,0))</f>
         <v>80</v>
       </c>
     </row>
@@ -5205,7 +7137,7 @@
         <v>407</v>
       </c>
       <c r="E55">
-        <f>IF(ISERROR(B55),"",MATCH(C55,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B55),"",MATCH(C55,Sheet!$A$2:$A$118,0))</f>
         <v>81</v>
       </c>
     </row>
@@ -5221,7 +7153,7 @@
         <v>408</v>
       </c>
       <c r="E56">
-        <f>IF(ISERROR(B56),"",MATCH(C56,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B56),"",MATCH(C56,Sheet!$A$2:$A$118,0))</f>
         <v>82</v>
       </c>
     </row>
@@ -5237,7 +7169,7 @@
         <v>409</v>
       </c>
       <c r="E57">
-        <f>IF(ISERROR(B57),"",MATCH(C57,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B57),"",MATCH(C57,Sheet!$A$2:$A$118,0))</f>
         <v>83</v>
       </c>
     </row>
@@ -5253,7 +7185,7 @@
         <v>410</v>
       </c>
       <c r="E58">
-        <f>IF(ISERROR(B58),"",MATCH(C58,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B58),"",MATCH(C58,Sheet!$A$2:$A$118,0))</f>
         <v>84</v>
       </c>
     </row>
@@ -5269,7 +7201,7 @@
         <v>411</v>
       </c>
       <c r="E59">
-        <f>IF(ISERROR(B59),"",MATCH(C59,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B59),"",MATCH(C59,Sheet!$A$2:$A$118,0))</f>
         <v>85</v>
       </c>
     </row>
@@ -5285,7 +7217,7 @@
         <v>412</v>
       </c>
       <c r="E60">
-        <f>IF(ISERROR(B60),"",MATCH(C60,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B60),"",MATCH(C60,Sheet!$A$2:$A$118,0))</f>
         <v>86</v>
       </c>
     </row>
@@ -5301,7 +7233,7 @@
         <v>413</v>
       </c>
       <c r="E61">
-        <f>IF(ISERROR(B61),"",MATCH(C61,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B61),"",MATCH(C61,Sheet!$A$2:$A$118,0))</f>
         <v>87</v>
       </c>
     </row>
@@ -5317,7 +7249,7 @@
         <v>414</v>
       </c>
       <c r="E62">
-        <f>IF(ISERROR(B62),"",MATCH(C62,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B62),"",MATCH(C62,Sheet!$A$2:$A$118,0))</f>
         <v>88</v>
       </c>
     </row>
@@ -5333,7 +7265,7 @@
         <v>415</v>
       </c>
       <c r="E63">
-        <f>IF(ISERROR(B63),"",MATCH(C63,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B63),"",MATCH(C63,Sheet!$A$2:$A$118,0))</f>
         <v>89</v>
       </c>
     </row>
@@ -5349,7 +7281,7 @@
         <v>416</v>
       </c>
       <c r="E64">
-        <f>IF(ISERROR(B64),"",MATCH(C64,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B64),"",MATCH(C64,Sheet!$A$2:$A$118,0))</f>
         <v>90</v>
       </c>
     </row>
@@ -5365,7 +7297,7 @@
         <v>417</v>
       </c>
       <c r="E65">
-        <f>IF(ISERROR(B65),"",MATCH(C65,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B65),"",MATCH(C65,Sheet!$A$2:$A$118,0))</f>
         <v>91</v>
       </c>
     </row>
@@ -5381,7 +7313,7 @@
         <v>418</v>
       </c>
       <c r="E66">
-        <f>IF(ISERROR(B66),"",MATCH(C66,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B66),"",MATCH(C66,Sheet!$A$2:$A$118,0))</f>
         <v>92</v>
       </c>
     </row>
@@ -5397,7 +7329,7 @@
         <v>419</v>
       </c>
       <c r="E67">
-        <f>IF(ISERROR(B67),"",MATCH(C67,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B67),"",MATCH(C67,Sheet!$A$2:$A$118,0))</f>
         <v>93</v>
       </c>
     </row>
@@ -5413,7 +7345,7 @@
         <v>420</v>
       </c>
       <c r="E68">
-        <f>IF(ISERROR(B68),"",MATCH(C68,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B68),"",MATCH(C68,Sheet!$A$2:$A$118,0))</f>
         <v>94</v>
       </c>
     </row>
@@ -5429,7 +7361,7 @@
         <v>421</v>
       </c>
       <c r="E69">
-        <f>IF(ISERROR(B69),"",MATCH(C69,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B69),"",MATCH(C69,Sheet!$A$2:$A$118,0))</f>
         <v>95</v>
       </c>
     </row>
@@ -5445,7 +7377,7 @@
         <v>422</v>
       </c>
       <c r="E70">
-        <f>IF(ISERROR(B70),"",MATCH(C70,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B70),"",MATCH(C70,Sheet!$A$2:$A$118,0))</f>
         <v>96</v>
       </c>
     </row>
@@ -5461,7 +7393,7 @@
         <v>423</v>
       </c>
       <c r="E71">
-        <f>IF(ISERROR(B71),"",MATCH(C71,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B71),"",MATCH(C71,Sheet!$A$2:$A$118,0))</f>
         <v>97</v>
       </c>
     </row>
@@ -5477,7 +7409,7 @@
         <v>424</v>
       </c>
       <c r="E72">
-        <f>IF(ISERROR(B72),"",MATCH(C72,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B72),"",MATCH(C72,Sheet!$A$2:$A$118,0))</f>
         <v>99</v>
       </c>
     </row>
@@ -5493,7 +7425,7 @@
         <v>425</v>
       </c>
       <c r="E73">
-        <f>IF(ISERROR(B73),"",MATCH(C73,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B73),"",MATCH(C73,Sheet!$A$2:$A$118,0))</f>
         <v>100</v>
       </c>
     </row>
@@ -5509,7 +7441,7 @@
         <v>426</v>
       </c>
       <c r="E74">
-        <f>IF(ISERROR(B74),"",MATCH(C74,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B74),"",MATCH(C74,Sheet!$A$2:$A$118,0))</f>
         <v>101</v>
       </c>
     </row>
@@ -5525,7 +7457,7 @@
         <v>427</v>
       </c>
       <c r="E75">
-        <f>IF(ISERROR(B75),"",MATCH(C75,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B75),"",MATCH(C75,Sheet!$A$2:$A$118,0))</f>
         <v>102</v>
       </c>
     </row>
@@ -5541,7 +7473,7 @@
         <v>428</v>
       </c>
       <c r="E76">
-        <f>IF(ISERROR(B76),"",MATCH(C76,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B76),"",MATCH(C76,Sheet!$A$2:$A$118,0))</f>
         <v>103</v>
       </c>
     </row>
@@ -5557,7 +7489,7 @@
         <v>429</v>
       </c>
       <c r="E77">
-        <f>IF(ISERROR(B77),"",MATCH(C77,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B77),"",MATCH(C77,Sheet!$A$2:$A$118,0))</f>
         <v>104</v>
       </c>
     </row>
@@ -5573,7 +7505,7 @@
         <v>430</v>
       </c>
       <c r="E78">
-        <f>IF(ISERROR(B78),"",MATCH(C78,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B78),"",MATCH(C78,Sheet!$A$2:$A$118,0))</f>
         <v>78</v>
       </c>
     </row>
@@ -5589,7 +7521,7 @@
         <v>431</v>
       </c>
       <c r="E79">
-        <f>IF(ISERROR(B79),"",MATCH(C79,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B79),"",MATCH(C79,Sheet!$A$2:$A$118,0))</f>
         <v>98</v>
       </c>
     </row>
@@ -5605,7 +7537,7 @@
         <v>432</v>
       </c>
       <c r="E80">
-        <f>IF(ISERROR(B80),"",MATCH(C80,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B80),"",MATCH(C80,Sheet!$A$2:$A$118,0))</f>
         <v>105</v>
       </c>
     </row>
@@ -5621,7 +7553,7 @@
         <v>433</v>
       </c>
       <c r="E81">
-        <f>IF(ISERROR(B81),"",MATCH(C81,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B81),"",MATCH(C81,Sheet!$A$2:$A$118,0))</f>
         <v>106</v>
       </c>
     </row>
@@ -5637,7 +7569,7 @@
         <v>434</v>
       </c>
       <c r="E82">
-        <f>IF(ISERROR(B82),"",MATCH(C82,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B82),"",MATCH(C82,Sheet!$A$2:$A$118,0))</f>
         <v>107</v>
       </c>
     </row>
@@ -5653,7 +7585,7 @@
         <v>435</v>
       </c>
       <c r="E83">
-        <f>IF(ISERROR(B83),"",MATCH(C83,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B83),"",MATCH(C83,Sheet!$A$2:$A$118,0))</f>
         <v>108</v>
       </c>
     </row>
@@ -5669,7 +7601,7 @@
         <v>436</v>
       </c>
       <c r="E84">
-        <f>IF(ISERROR(B84),"",MATCH(C84,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B84),"",MATCH(C84,Sheet!$A$2:$A$118,0))</f>
         <v>109</v>
       </c>
     </row>
@@ -5685,8 +7617,8 @@
         <v>437</v>
       </c>
       <c r="E85">
-        <f>IF(ISERROR(B85),"",MATCH(C85,Sheet!$A$2:$A$115,0))</f>
-        <v>110</v>
+        <f>IF(ISERROR(B85),"",MATCH(C85,Sheet!$A$2:$A$118,0))</f>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.45">
@@ -5701,8 +7633,8 @@
         <v>438</v>
       </c>
       <c r="E86">
-        <f>IF(ISERROR(B86),"",MATCH(C86,Sheet!$A$2:$A$115,0))</f>
-        <v>111</v>
+        <f>IF(ISERROR(B86),"",MATCH(C86,Sheet!$A$2:$A$118,0))</f>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.45">
@@ -5717,8 +7649,8 @@
         <v>439</v>
       </c>
       <c r="E87">
-        <f>IF(ISERROR(B87),"",MATCH(C87,Sheet!$A$2:$A$115,0))</f>
-        <v>112</v>
+        <f>IF(ISERROR(B87),"",MATCH(C87,Sheet!$A$2:$A$118,0))</f>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.45">
@@ -5733,8 +7665,8 @@
         <v>440</v>
       </c>
       <c r="E88">
-        <f>IF(ISERROR(B88),"",MATCH(C88,Sheet!$A$2:$A$115,0))</f>
-        <v>113</v>
+        <f>IF(ISERROR(B88),"",MATCH(C88,Sheet!$A$2:$A$118,0))</f>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.45">
@@ -5749,8 +7681,8 @@
         <v>441</v>
       </c>
       <c r="E89">
-        <f>IF(ISERROR(B89),"",MATCH(C89,Sheet!$A$2:$A$115,0))</f>
-        <v>114</v>
+        <f>IF(ISERROR(B89),"",MATCH(C89,Sheet!$A$2:$A$118,0))</f>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.45">
@@ -5765,7 +7697,7 @@
         <v>442</v>
       </c>
       <c r="E90">
-        <f>IF(ISERROR(B90),"",MATCH(C90,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B90),"",MATCH(C90,Sheet!$A$2:$A$118,0))</f>
         <v>1</v>
       </c>
     </row>
@@ -5781,7 +7713,7 @@
         <v>443</v>
       </c>
       <c r="E91">
-        <f>IF(ISERROR(B91),"",MATCH(C91,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B91),"",MATCH(C91,Sheet!$A$2:$A$118,0))</f>
         <v>2</v>
       </c>
     </row>
@@ -5797,7 +7729,7 @@
         <v>444</v>
       </c>
       <c r="E92">
-        <f>IF(ISERROR(B92),"",MATCH(C92,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B92),"",MATCH(C92,Sheet!$A$2:$A$118,0))</f>
         <v>3</v>
       </c>
     </row>
@@ -5813,7 +7745,7 @@
         <v>445</v>
       </c>
       <c r="E93">
-        <f>IF(ISERROR(B93),"",MATCH(C93,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B93),"",MATCH(C93,Sheet!$A$2:$A$118,0))</f>
         <v>4</v>
       </c>
     </row>
@@ -5829,7 +7761,7 @@
         <v>446</v>
       </c>
       <c r="E94">
-        <f>IF(ISERROR(B94),"",MATCH(C94,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B94),"",MATCH(C94,Sheet!$A$2:$A$118,0))</f>
         <v>5</v>
       </c>
     </row>
@@ -5845,7 +7777,7 @@
         <v>447</v>
       </c>
       <c r="E95">
-        <f>IF(ISERROR(B95),"",MATCH(C95,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B95),"",MATCH(C95,Sheet!$A$2:$A$118,0))</f>
         <v>6</v>
       </c>
     </row>
@@ -5861,7 +7793,7 @@
         <v>448</v>
       </c>
       <c r="E96">
-        <f>IF(ISERROR(B96),"",MATCH(C96,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B96),"",MATCH(C96,Sheet!$A$2:$A$118,0))</f>
         <v>7</v>
       </c>
     </row>
@@ -5877,7 +7809,7 @@
         <v>449</v>
       </c>
       <c r="E97">
-        <f>IF(ISERROR(B97),"",MATCH(C97,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B97),"",MATCH(C97,Sheet!$A$2:$A$118,0))</f>
         <v>8</v>
       </c>
     </row>
@@ -5893,7 +7825,7 @@
         <v>450</v>
       </c>
       <c r="E98">
-        <f>IF(ISERROR(B98),"",MATCH(C98,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B98),"",MATCH(C98,Sheet!$A$2:$A$118,0))</f>
         <v>9</v>
       </c>
     </row>
@@ -5909,7 +7841,7 @@
         <v>451</v>
       </c>
       <c r="E99">
-        <f>IF(ISERROR(B99),"",MATCH(C99,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B99),"",MATCH(C99,Sheet!$A$2:$A$118,0))</f>
         <v>10</v>
       </c>
     </row>
@@ -5925,7 +7857,7 @@
         <v>43</v>
       </c>
       <c r="E100">
-        <f>IF(ISERROR(B100),"",MATCH(C100,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B100),"",MATCH(C100,Sheet!$A$2:$A$118,0))</f>
         <v>11</v>
       </c>
     </row>
@@ -5941,7 +7873,7 @@
         <v>452</v>
       </c>
       <c r="E101">
-        <f>IF(ISERROR(B101),"",MATCH(C101,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B101),"",MATCH(C101,Sheet!$A$2:$A$118,0))</f>
         <v>12</v>
       </c>
     </row>
@@ -5957,7 +7889,7 @@
         <v>49</v>
       </c>
       <c r="E102">
-        <f>IF(ISERROR(B102),"",MATCH(C102,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B102),"",MATCH(C102,Sheet!$A$2:$A$118,0))</f>
         <v>13</v>
       </c>
     </row>
@@ -5973,7 +7905,7 @@
         <v>453</v>
       </c>
       <c r="E103">
-        <f>IF(ISERROR(B103),"",MATCH(C103,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B103),"",MATCH(C103,Sheet!$A$2:$A$118,0))</f>
         <v>14</v>
       </c>
     </row>
@@ -5989,7 +7921,7 @@
         <v>55</v>
       </c>
       <c r="E104">
-        <f>IF(ISERROR(B104),"",MATCH(C104,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B104),"",MATCH(C104,Sheet!$A$2:$A$118,0))</f>
         <v>15</v>
       </c>
     </row>
@@ -6005,7 +7937,7 @@
         <v>454</v>
       </c>
       <c r="E105">
-        <f>IF(ISERROR(B105),"",MATCH(C105,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B105),"",MATCH(C105,Sheet!$A$2:$A$118,0))</f>
         <v>16</v>
       </c>
     </row>
@@ -6021,7 +7953,7 @@
         <v>455</v>
       </c>
       <c r="E106">
-        <f>IF(ISERROR(B106),"",MATCH(C106,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B106),"",MATCH(C106,Sheet!$A$2:$A$118,0))</f>
         <v>19</v>
       </c>
     </row>
@@ -6037,7 +7969,7 @@
         <v>456</v>
       </c>
       <c r="E107">
-        <f>IF(ISERROR(B107),"",MATCH(C107,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B107),"",MATCH(C107,Sheet!$A$2:$A$118,0))</f>
         <v>20</v>
       </c>
     </row>
@@ -6053,7 +7985,7 @@
         <v>457</v>
       </c>
       <c r="E108">
-        <f>IF(ISERROR(B108),"",MATCH(C108,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B108),"",MATCH(C108,Sheet!$A$2:$A$118,0))</f>
         <v>21</v>
       </c>
     </row>
@@ -6069,7 +8001,7 @@
         <v>458</v>
       </c>
       <c r="E109">
-        <f>IF(ISERROR(B109),"",MATCH(C109,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B109),"",MATCH(C109,Sheet!$A$2:$A$118,0))</f>
         <v>22</v>
       </c>
     </row>
@@ -6085,7 +8017,7 @@
         <v>459</v>
       </c>
       <c r="E110">
-        <f>IF(ISERROR(B110),"",MATCH(C110,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B110),"",MATCH(C110,Sheet!$A$2:$A$118,0))</f>
         <v>25</v>
       </c>
     </row>
@@ -6101,7 +8033,7 @@
         <v>460</v>
       </c>
       <c r="E111">
-        <f>IF(ISERROR(B111),"",MATCH(C111,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B111),"",MATCH(C111,Sheet!$A$2:$A$118,0))</f>
         <v>26</v>
       </c>
     </row>
@@ -6117,7 +8049,7 @@
         <v>61</v>
       </c>
       <c r="E112">
-        <f>IF(ISERROR(B112),"",MATCH(C112,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B112),"",MATCH(C112,Sheet!$A$2:$A$118,0))</f>
         <v>17</v>
       </c>
     </row>
@@ -6133,7 +8065,7 @@
         <v>461</v>
       </c>
       <c r="E113">
-        <f>IF(ISERROR(B113),"",MATCH(C113,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B113),"",MATCH(C113,Sheet!$A$2:$A$118,0))</f>
         <v>18</v>
       </c>
     </row>
@@ -6149,7 +8081,7 @@
         <v>462</v>
       </c>
       <c r="E114">
-        <f>IF(ISERROR(B114),"",MATCH(C114,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B114),"",MATCH(C114,Sheet!$A$2:$A$118,0))</f>
         <v>23</v>
       </c>
     </row>
@@ -6165,7 +8097,7 @@
         <v>463</v>
       </c>
       <c r="E115">
-        <f>IF(ISERROR(B115),"",MATCH(C115,Sheet!$A$2:$A$115,0))</f>
+        <f>IF(ISERROR(B115),"",MATCH(C115,Sheet!$A$2:$A$118,0))</f>
         <v>24</v>
       </c>
     </row>

</xml_diff>